<commit_message>
Finished full test and excel generation
</commit_message>
<xml_diff>
--- a/PROJECT/Output.xlsx
+++ b/PROJECT/Output.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="2970" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="13959" uniqueCount="99">
   <si>
     <t>NOM</t>
   </si>
@@ -918,8 +918,12 @@
       <c r="C33" s="0">
         <v>1</v>
       </c>
-      <c r="D33" s="0"/>
-      <c r="E33" s="0"/>
+      <c r="D33" s="0">
+        <v>1</v>
+      </c>
+      <c r="E33" s="0">
+        <v>1</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="0" t="s">
@@ -931,8 +935,12 @@
       <c r="C34" s="0">
         <v>1</v>
       </c>
-      <c r="D34" s="0"/>
-      <c r="E34" s="0"/>
+      <c r="D34" s="0">
+        <v>0</v>
+      </c>
+      <c r="E34" s="0">
+        <v>1</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="0" t="s">
@@ -944,8 +952,12 @@
       <c r="C35" s="0">
         <v>0</v>
       </c>
-      <c r="D35" s="0"/>
-      <c r="E35" s="0"/>
+      <c r="D35" s="0">
+        <v>0</v>
+      </c>
+      <c r="E35" s="0">
+        <v>1</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="0" t="s">
@@ -957,8 +969,12 @@
       <c r="C36" s="0">
         <v>1</v>
       </c>
-      <c r="D36" s="0"/>
-      <c r="E36" s="0"/>
+      <c r="D36" s="0">
+        <v>0</v>
+      </c>
+      <c r="E36" s="0">
+        <v>1</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="0" t="s">
@@ -970,8 +986,12 @@
       <c r="C37" s="0">
         <v>1</v>
       </c>
-      <c r="D37" s="0"/>
-      <c r="E37" s="0"/>
+      <c r="D37" s="0">
+        <v>0</v>
+      </c>
+      <c r="E37" s="0">
+        <v>1</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="0" t="s">
@@ -983,8 +1003,12 @@
       <c r="C38" s="0">
         <v>1</v>
       </c>
-      <c r="D38" s="0"/>
-      <c r="E38" s="0"/>
+      <c r="D38" s="0">
+        <v>1</v>
+      </c>
+      <c r="E38" s="0">
+        <v>1</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="0" t="s">
@@ -996,8 +1020,12 @@
       <c r="C39" s="0">
         <v>0</v>
       </c>
-      <c r="D39" s="0"/>
-      <c r="E39" s="0"/>
+      <c r="D39" s="0">
+        <v>0</v>
+      </c>
+      <c r="E39" s="0">
+        <v>0</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="0" t="s">
@@ -1009,8 +1037,12 @@
       <c r="C40" s="0">
         <v>0</v>
       </c>
-      <c r="D40" s="0"/>
-      <c r="E40" s="0"/>
+      <c r="D40" s="0">
+        <v>1</v>
+      </c>
+      <c r="E40" s="0">
+        <v>0</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="0" t="s">
@@ -1022,8 +1054,12 @@
       <c r="C41" s="0">
         <v>0</v>
       </c>
-      <c r="D41" s="0"/>
-      <c r="E41" s="0"/>
+      <c r="D41" s="0">
+        <v>1</v>
+      </c>
+      <c r="E41" s="0">
+        <v>1</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="0" t="s">
@@ -1035,8 +1071,12 @@
       <c r="C42" s="0">
         <v>0</v>
       </c>
-      <c r="D42" s="0"/>
-      <c r="E42" s="0"/>
+      <c r="D42" s="0">
+        <v>0</v>
+      </c>
+      <c r="E42" s="0">
+        <v>1</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="0" t="s">
@@ -1048,8 +1088,12 @@
       <c r="C43" s="0">
         <v>0</v>
       </c>
-      <c r="D43" s="0"/>
-      <c r="E43" s="0"/>
+      <c r="D43" s="0">
+        <v>0</v>
+      </c>
+      <c r="E43" s="0">
+        <v>0</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="0" t="s">
@@ -1061,8 +1105,12 @@
       <c r="C44" s="0">
         <v>0</v>
       </c>
-      <c r="D44" s="0"/>
-      <c r="E44" s="0"/>
+      <c r="D44" s="0">
+        <v>1</v>
+      </c>
+      <c r="E44" s="0">
+        <v>1</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="0" t="s">
@@ -1074,8 +1122,12 @@
       <c r="C45" s="0">
         <v>0</v>
       </c>
-      <c r="D45" s="0"/>
-      <c r="E45" s="0"/>
+      <c r="D45" s="0">
+        <v>0</v>
+      </c>
+      <c r="E45" s="0">
+        <v>0</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" s="0" t="s">
@@ -1087,8 +1139,12 @@
       <c r="C46" s="0">
         <v>0</v>
       </c>
-      <c r="D46" s="0"/>
-      <c r="E46" s="0"/>
+      <c r="D46" s="0">
+        <v>0</v>
+      </c>
+      <c r="E46" s="0">
+        <v>1</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="0" t="s">
@@ -1100,8 +1156,12 @@
       <c r="C47" s="0">
         <v>0</v>
       </c>
-      <c r="D47" s="0"/>
-      <c r="E47" s="0"/>
+      <c r="D47" s="0">
+        <v>1</v>
+      </c>
+      <c r="E47" s="0">
+        <v>0</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" s="0" t="s">
@@ -1113,8 +1173,12 @@
       <c r="C48" s="0">
         <v>0</v>
       </c>
-      <c r="D48" s="0"/>
-      <c r="E48" s="0"/>
+      <c r="D48" s="0">
+        <v>1</v>
+      </c>
+      <c r="E48" s="0">
+        <v>1</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" s="0" t="s">
@@ -1126,8 +1190,12 @@
       <c r="C49" s="0">
         <v>0</v>
       </c>
-      <c r="D49" s="0"/>
-      <c r="E49" s="0"/>
+      <c r="D49" s="0">
+        <v>1</v>
+      </c>
+      <c r="E49" s="0">
+        <v>1</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="0" t="s">
@@ -1139,8 +1207,12 @@
       <c r="C50" s="0">
         <v>0</v>
       </c>
-      <c r="D50" s="0"/>
-      <c r="E50" s="0"/>
+      <c r="D50" s="0">
+        <v>1</v>
+      </c>
+      <c r="E50" s="0">
+        <v>0</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" s="0" t="s">
@@ -1152,8 +1224,12 @@
       <c r="C51" s="0">
         <v>0</v>
       </c>
-      <c r="D51" s="0"/>
-      <c r="E51" s="0"/>
+      <c r="D51" s="0">
+        <v>1</v>
+      </c>
+      <c r="E51" s="0">
+        <v>1</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" s="0" t="s">
@@ -1165,8 +1241,12 @@
       <c r="C52" s="0">
         <v>0</v>
       </c>
-      <c r="D52" s="0"/>
-      <c r="E52" s="0"/>
+      <c r="D52" s="0">
+        <v>0</v>
+      </c>
+      <c r="E52" s="0">
+        <v>0</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" s="0" t="s">
@@ -1178,8 +1258,12 @@
       <c r="C53" s="0">
         <v>0</v>
       </c>
-      <c r="D53" s="0"/>
-      <c r="E53" s="0"/>
+      <c r="D53" s="0">
+        <v>0</v>
+      </c>
+      <c r="E53" s="0">
+        <v>0</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" s="0" t="s">
@@ -1191,8 +1275,12 @@
       <c r="C54" s="0">
         <v>0</v>
       </c>
-      <c r="D54" s="0"/>
-      <c r="E54" s="0"/>
+      <c r="D54" s="0">
+        <v>1</v>
+      </c>
+      <c r="E54" s="0">
+        <v>1</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" s="0" t="s">
@@ -1204,8 +1292,12 @@
       <c r="C55" s="0">
         <v>0</v>
       </c>
-      <c r="D55" s="0"/>
-      <c r="E55" s="0"/>
+      <c r="D55" s="0">
+        <v>0</v>
+      </c>
+      <c r="E55" s="0">
+        <v>0</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" s="0" t="s">
@@ -1217,8 +1309,12 @@
       <c r="C56" s="0">
         <v>0</v>
       </c>
-      <c r="D56" s="0"/>
-      <c r="E56" s="0"/>
+      <c r="D56" s="0">
+        <v>0</v>
+      </c>
+      <c r="E56" s="0">
+        <v>0</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" s="0" t="s">
@@ -1230,8 +1326,12 @@
       <c r="C57" s="0">
         <v>0</v>
       </c>
-      <c r="D57" s="0"/>
-      <c r="E57" s="0"/>
+      <c r="D57" s="0">
+        <v>0</v>
+      </c>
+      <c r="E57" s="0">
+        <v>1</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" s="0" t="s">
@@ -1243,8 +1343,12 @@
       <c r="C58" s="0">
         <v>0</v>
       </c>
-      <c r="D58" s="0"/>
-      <c r="E58" s="0"/>
+      <c r="D58" s="0">
+        <v>0</v>
+      </c>
+      <c r="E58" s="0">
+        <v>0</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" s="0" t="s">
@@ -1256,8 +1360,12 @@
       <c r="C59" s="0">
         <v>0</v>
       </c>
-      <c r="D59" s="0"/>
-      <c r="E59" s="0"/>
+      <c r="D59" s="0">
+        <v>1</v>
+      </c>
+      <c r="E59" s="0">
+        <v>1</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" s="0" t="s">
@@ -1269,8 +1377,12 @@
       <c r="C60" s="0">
         <v>0</v>
       </c>
-      <c r="D60" s="0"/>
-      <c r="E60" s="0"/>
+      <c r="D60" s="0">
+        <v>1</v>
+      </c>
+      <c r="E60" s="0">
+        <v>0</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" s="0" t="s">
@@ -1282,8 +1394,12 @@
       <c r="C61" s="0">
         <v>1</v>
       </c>
-      <c r="D61" s="0"/>
-      <c r="E61" s="0"/>
+      <c r="D61" s="0">
+        <v>0</v>
+      </c>
+      <c r="E61" s="0">
+        <v>1</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" s="0" t="s">
@@ -1295,8 +1411,12 @@
       <c r="C62" s="0">
         <v>0</v>
       </c>
-      <c r="D62" s="0"/>
-      <c r="E62" s="0"/>
+      <c r="D62" s="0">
+        <v>1</v>
+      </c>
+      <c r="E62" s="0">
+        <v>0</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" s="0" t="s">
@@ -1308,8 +1428,12 @@
       <c r="C63" s="0">
         <v>0</v>
       </c>
-      <c r="D63" s="0"/>
-      <c r="E63" s="0"/>
+      <c r="D63" s="0">
+        <v>1</v>
+      </c>
+      <c r="E63" s="0">
+        <v>1</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" s="0" t="s">
@@ -1321,8 +1445,12 @@
       <c r="C64" s="0">
         <v>0</v>
       </c>
-      <c r="D64" s="0"/>
-      <c r="E64" s="0"/>
+      <c r="D64" s="0">
+        <v>1</v>
+      </c>
+      <c r="E64" s="0">
+        <v>0</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" s="0" t="s">
@@ -1334,8 +1462,12 @@
       <c r="C65" s="0">
         <v>0</v>
       </c>
-      <c r="D65" s="0"/>
-      <c r="E65" s="0"/>
+      <c r="D65" s="0">
+        <v>0</v>
+      </c>
+      <c r="E65" s="0">
+        <v>1</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" s="0" t="s">
@@ -1347,8 +1479,12 @@
       <c r="C66" s="0">
         <v>0</v>
       </c>
-      <c r="D66" s="0"/>
-      <c r="E66" s="0"/>
+      <c r="D66" s="0">
+        <v>0</v>
+      </c>
+      <c r="E66" s="0">
+        <v>0</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" s="0" t="s">
@@ -1360,8 +1496,12 @@
       <c r="C67" s="0">
         <v>0</v>
       </c>
-      <c r="D67" s="0"/>
-      <c r="E67" s="0"/>
+      <c r="D67" s="0">
+        <v>2</v>
+      </c>
+      <c r="E67" s="0">
+        <v>0</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" s="0" t="s">
@@ -1373,8 +1513,12 @@
       <c r="C68" s="0">
         <v>0</v>
       </c>
-      <c r="D68" s="0"/>
-      <c r="E68" s="0"/>
+      <c r="D68" s="0">
+        <v>1</v>
+      </c>
+      <c r="E68" s="0">
+        <v>0</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" s="0" t="s">
@@ -1386,8 +1530,12 @@
       <c r="C69" s="0">
         <v>0</v>
       </c>
-      <c r="D69" s="0"/>
-      <c r="E69" s="0"/>
+      <c r="D69" s="0">
+        <v>1</v>
+      </c>
+      <c r="E69" s="0">
+        <v>0</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" s="0" t="s">
@@ -1399,8 +1547,12 @@
       <c r="C70" s="0">
         <v>0</v>
       </c>
-      <c r="D70" s="0"/>
-      <c r="E70" s="0"/>
+      <c r="D70" s="0">
+        <v>0</v>
+      </c>
+      <c r="E70" s="0">
+        <v>0</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" s="0" t="s">
@@ -1412,8 +1564,12 @@
       <c r="C71" s="0">
         <v>0</v>
       </c>
-      <c r="D71" s="0"/>
-      <c r="E71" s="0"/>
+      <c r="D71" s="0">
+        <v>0</v>
+      </c>
+      <c r="E71" s="0">
+        <v>0</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" s="0" t="s">
@@ -1425,8 +1581,12 @@
       <c r="C72" s="0">
         <v>0</v>
       </c>
-      <c r="D72" s="0"/>
-      <c r="E72" s="0"/>
+      <c r="D72" s="0">
+        <v>0</v>
+      </c>
+      <c r="E72" s="0">
+        <v>1</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" s="0" t="s">
@@ -1438,8 +1598,12 @@
       <c r="C73" s="0">
         <v>0</v>
       </c>
-      <c r="D73" s="0"/>
-      <c r="E73" s="0"/>
+      <c r="D73" s="0">
+        <v>1</v>
+      </c>
+      <c r="E73" s="0">
+        <v>0</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" s="0" t="s">
@@ -1451,8 +1615,12 @@
       <c r="C74" s="0">
         <v>0</v>
       </c>
-      <c r="D74" s="0"/>
-      <c r="E74" s="0"/>
+      <c r="D74" s="0">
+        <v>1</v>
+      </c>
+      <c r="E74" s="0">
+        <v>1</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" s="0" t="s">
@@ -1464,8 +1632,12 @@
       <c r="C75" s="0">
         <v>0</v>
       </c>
-      <c r="D75" s="0"/>
-      <c r="E75" s="0"/>
+      <c r="D75" s="0">
+        <v>0</v>
+      </c>
+      <c r="E75" s="0">
+        <v>0</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" s="0" t="s">
@@ -1477,8 +1649,12 @@
       <c r="C76" s="0">
         <v>0</v>
       </c>
-      <c r="D76" s="0"/>
-      <c r="E76" s="0"/>
+      <c r="D76" s="0">
+        <v>0</v>
+      </c>
+      <c r="E76" s="0">
+        <v>0</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" s="0" t="s">
@@ -1490,8 +1666,12 @@
       <c r="C77" s="0">
         <v>0</v>
       </c>
-      <c r="D77" s="0"/>
-      <c r="E77" s="0"/>
+      <c r="D77" s="0">
+        <v>1</v>
+      </c>
+      <c r="E77" s="0">
+        <v>0</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" s="0" t="s">
@@ -1503,8 +1683,12 @@
       <c r="C78" s="0">
         <v>0</v>
       </c>
-      <c r="D78" s="0"/>
-      <c r="E78" s="0"/>
+      <c r="D78" s="0">
+        <v>0</v>
+      </c>
+      <c r="E78" s="0">
+        <v>1</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" s="0" t="s">
@@ -1516,8 +1700,12 @@
       <c r="C79" s="0">
         <v>0</v>
       </c>
-      <c r="D79" s="0"/>
-      <c r="E79" s="0"/>
+      <c r="D79" s="0">
+        <v>1</v>
+      </c>
+      <c r="E79" s="0">
+        <v>0</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" s="0" t="s">
@@ -1529,8 +1717,12 @@
       <c r="C80" s="0">
         <v>0</v>
       </c>
-      <c r="D80" s="0"/>
-      <c r="E80" s="0"/>
+      <c r="D80" s="0">
+        <v>1</v>
+      </c>
+      <c r="E80" s="0">
+        <v>0</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" s="0" t="s">
@@ -1542,8 +1734,12 @@
       <c r="C81" s="0">
         <v>0</v>
       </c>
-      <c r="D81" s="0"/>
-      <c r="E81" s="0"/>
+      <c r="D81" s="0">
+        <v>0</v>
+      </c>
+      <c r="E81" s="0">
+        <v>0</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" s="0" t="s">
@@ -1555,8 +1751,12 @@
       <c r="C82" s="0">
         <v>1</v>
       </c>
-      <c r="D82" s="0"/>
-      <c r="E82" s="0"/>
+      <c r="D82" s="0">
+        <v>0</v>
+      </c>
+      <c r="E82" s="0">
+        <v>1</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" s="0" t="s">
@@ -1568,8 +1768,12 @@
       <c r="C83" s="0">
         <v>1</v>
       </c>
-      <c r="D83" s="0"/>
-      <c r="E83" s="0"/>
+      <c r="D83" s="0">
+        <v>0</v>
+      </c>
+      <c r="E83" s="0">
+        <v>1</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" s="0" t="s">
@@ -1581,8 +1785,12 @@
       <c r="C84" s="0">
         <v>1</v>
       </c>
-      <c r="D84" s="0"/>
-      <c r="E84" s="0"/>
+      <c r="D84" s="0">
+        <v>0</v>
+      </c>
+      <c r="E84" s="0">
+        <v>1</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" s="0" t="s">
@@ -1594,8 +1802,12 @@
       <c r="C85" s="0">
         <v>1</v>
       </c>
-      <c r="D85" s="0"/>
-      <c r="E85" s="0"/>
+      <c r="D85" s="0">
+        <v>1</v>
+      </c>
+      <c r="E85" s="0">
+        <v>1</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" s="0" t="s">
@@ -1607,8 +1819,12 @@
       <c r="C86" s="0">
         <v>0</v>
       </c>
-      <c r="D86" s="0"/>
-      <c r="E86" s="0"/>
+      <c r="D86" s="0">
+        <v>0</v>
+      </c>
+      <c r="E86" s="0">
+        <v>0</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87" s="0" t="s">
@@ -1620,8 +1836,12 @@
       <c r="C87" s="0">
         <v>0</v>
       </c>
-      <c r="D87" s="0"/>
-      <c r="E87" s="0"/>
+      <c r="D87" s="0">
+        <v>1</v>
+      </c>
+      <c r="E87" s="0">
+        <v>0</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" s="0" t="s">
@@ -1633,8 +1853,12 @@
       <c r="C88" s="0">
         <v>0</v>
       </c>
-      <c r="D88" s="0"/>
-      <c r="E88" s="0"/>
+      <c r="D88" s="0">
+        <v>0</v>
+      </c>
+      <c r="E88" s="0">
+        <v>0</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89" s="0" t="s">
@@ -1646,8 +1870,12 @@
       <c r="C89" s="0">
         <v>0</v>
       </c>
-      <c r="D89" s="0"/>
-      <c r="E89" s="0"/>
+      <c r="D89" s="0">
+        <v>1</v>
+      </c>
+      <c r="E89" s="0">
+        <v>1</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90" s="0" t="s">
@@ -1659,8 +1887,12 @@
       <c r="C90" s="0">
         <v>0</v>
       </c>
-      <c r="D90" s="0"/>
-      <c r="E90" s="0"/>
+      <c r="D90" s="0">
+        <v>1</v>
+      </c>
+      <c r="E90" s="0">
+        <v>1</v>
+      </c>
     </row>
     <row r="91">
       <c r="A91" s="0" t="s">
@@ -1672,8 +1904,12 @@
       <c r="C91" s="0">
         <v>0</v>
       </c>
-      <c r="D91" s="0"/>
-      <c r="E91" s="0"/>
+      <c r="D91" s="0">
+        <v>1</v>
+      </c>
+      <c r="E91" s="0">
+        <v>1</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92" s="0" t="s">
@@ -1685,8 +1921,12 @@
       <c r="C92" s="0">
         <v>0</v>
       </c>
-      <c r="D92" s="0"/>
-      <c r="E92" s="0"/>
+      <c r="D92" s="0">
+        <v>1</v>
+      </c>
+      <c r="E92" s="0">
+        <v>0</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93" s="0" t="s">
@@ -1698,8 +1938,12 @@
       <c r="C93" s="0">
         <v>0</v>
       </c>
-      <c r="D93" s="0"/>
-      <c r="E93" s="0"/>
+      <c r="D93" s="0">
+        <v>1</v>
+      </c>
+      <c r="E93" s="0">
+        <v>1</v>
+      </c>
     </row>
     <row r="94">
       <c r="A94" s="0" t="s">
@@ -1711,8 +1955,12 @@
       <c r="C94" s="0">
         <v>0</v>
       </c>
-      <c r="D94" s="0"/>
-      <c r="E94" s="0"/>
+      <c r="D94" s="0">
+        <v>0</v>
+      </c>
+      <c r="E94" s="0">
+        <v>1</v>
+      </c>
     </row>
     <row r="95">
       <c r="A95" s="0" t="s">

</xml_diff>

<commit_message>
Final Detection fully validated
</commit_message>
<xml_diff>
--- a/PROJECT/Output.xlsx
+++ b/PROJECT/Output.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="13959" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="14751" uniqueCount="99">
   <si>
     <t>NOM</t>
   </si>
@@ -361,11 +361,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="43" customWidth="true"/>
-    <col min="2" max="2" width="5.7109375" customWidth="true"/>
-    <col min="3" max="3" width="5.85546875" customWidth="true"/>
-    <col min="4" max="4" width="11.85546875" customWidth="true"/>
-    <col min="5" max="5" width="11.85546875" customWidth="true"/>
+    <col min="1" max="1" width="40.6640625" customWidth="true"/>
+    <col min="2" max="2" width="5.21875" customWidth="true"/>
+    <col min="3" max="3" width="5.44140625" customWidth="true"/>
+    <col min="4" max="4" width="11.44140625" customWidth="true"/>
+    <col min="5" max="5" width="11.5546875" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -409,7 +409,7 @@
         <v>0</v>
       </c>
       <c r="D3" s="0">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3" s="0">
         <v>0</v>
@@ -494,7 +494,7 @@
         <v>0</v>
       </c>
       <c r="D8" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E8" s="0">
         <v>0</v>
@@ -531,7 +531,7 @@
         <v>0</v>
       </c>
       <c r="E10" s="0">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11">
@@ -616,7 +616,7 @@
         <v>3</v>
       </c>
       <c r="E15" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
@@ -647,7 +647,7 @@
         <v>0</v>
       </c>
       <c r="D17" s="0">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E17" s="0">
         <v>0</v>
@@ -667,7 +667,7 @@
         <v>0</v>
       </c>
       <c r="E18" s="0">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19">
@@ -681,7 +681,7 @@
         <v>0</v>
       </c>
       <c r="D19" s="0">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E19" s="0">
         <v>0</v>
@@ -701,7 +701,7 @@
         <v>0</v>
       </c>
       <c r="E20" s="0">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21">
@@ -731,12 +731,8 @@
       <c r="C22" s="0">
         <v>1</v>
       </c>
-      <c r="D22" s="0">
-        <v>0</v>
-      </c>
-      <c r="E22" s="0">
-        <v>1</v>
-      </c>
+      <c r="D22" s="0"/>
+      <c r="E22" s="0"/>
     </row>
     <row r="23">
       <c r="A23" s="0" t="s">
@@ -748,12 +744,8 @@
       <c r="C23" s="0">
         <v>0</v>
       </c>
-      <c r="D23" s="0">
-        <v>0</v>
-      </c>
-      <c r="E23" s="0">
-        <v>0</v>
-      </c>
+      <c r="D23" s="0"/>
+      <c r="E23" s="0"/>
     </row>
     <row r="24">
       <c r="A24" s="0" t="s">
@@ -765,12 +757,8 @@
       <c r="C24" s="0">
         <v>0</v>
       </c>
-      <c r="D24" s="0">
-        <v>0</v>
-      </c>
-      <c r="E24" s="0">
-        <v>0</v>
-      </c>
+      <c r="D24" s="0"/>
+      <c r="E24" s="0"/>
     </row>
     <row r="25">
       <c r="A25" s="0" t="s">
@@ -782,12 +770,8 @@
       <c r="C25" s="0">
         <v>0</v>
       </c>
-      <c r="D25" s="0">
-        <v>0</v>
-      </c>
-      <c r="E25" s="0">
-        <v>1</v>
-      </c>
+      <c r="D25" s="0"/>
+      <c r="E25" s="0"/>
     </row>
     <row r="26">
       <c r="A26" s="0" t="s">
@@ -799,12 +783,8 @@
       <c r="C26" s="0">
         <v>1</v>
       </c>
-      <c r="D26" s="0">
-        <v>0</v>
-      </c>
-      <c r="E26" s="0">
-        <v>1</v>
-      </c>
+      <c r="D26" s="0"/>
+      <c r="E26" s="0"/>
     </row>
     <row r="27">
       <c r="A27" s="0" t="s">
@@ -816,12 +796,8 @@
       <c r="C27" s="0">
         <v>1</v>
       </c>
-      <c r="D27" s="0">
-        <v>0</v>
-      </c>
-      <c r="E27" s="0">
-        <v>2</v>
-      </c>
+      <c r="D27" s="0"/>
+      <c r="E27" s="0"/>
     </row>
     <row r="28">
       <c r="A28" s="0" t="s">
@@ -833,12 +809,8 @@
       <c r="C28" s="0">
         <v>0</v>
       </c>
-      <c r="D28" s="0">
-        <v>1</v>
-      </c>
-      <c r="E28" s="0">
-        <v>0</v>
-      </c>
+      <c r="D28" s="0"/>
+      <c r="E28" s="0"/>
     </row>
     <row r="29">
       <c r="A29" s="0" t="s">
@@ -850,12 +822,8 @@
       <c r="C29" s="0">
         <v>1</v>
       </c>
-      <c r="D29" s="0">
-        <v>0</v>
-      </c>
-      <c r="E29" s="0">
-        <v>0</v>
-      </c>
+      <c r="D29" s="0"/>
+      <c r="E29" s="0"/>
     </row>
     <row r="30">
       <c r="A30" s="0" t="s">
@@ -867,12 +835,8 @@
       <c r="C30" s="0">
         <v>1</v>
       </c>
-      <c r="D30" s="0">
-        <v>0</v>
-      </c>
-      <c r="E30" s="0">
-        <v>1</v>
-      </c>
+      <c r="D30" s="0"/>
+      <c r="E30" s="0"/>
     </row>
     <row r="31">
       <c r="A31" s="0" t="s">
@@ -884,12 +848,8 @@
       <c r="C31" s="0">
         <v>1</v>
       </c>
-      <c r="D31" s="0">
-        <v>0</v>
-      </c>
-      <c r="E31" s="0">
-        <v>1</v>
-      </c>
+      <c r="D31" s="0"/>
+      <c r="E31" s="0"/>
     </row>
     <row r="32">
       <c r="A32" s="0" t="s">
@@ -901,12 +861,8 @@
       <c r="C32" s="0">
         <v>1</v>
       </c>
-      <c r="D32" s="0">
-        <v>0</v>
-      </c>
-      <c r="E32" s="0">
-        <v>0</v>
-      </c>
+      <c r="D32" s="0"/>
+      <c r="E32" s="0"/>
     </row>
     <row r="33">
       <c r="A33" s="0" t="s">
@@ -918,12 +874,8 @@
       <c r="C33" s="0">
         <v>1</v>
       </c>
-      <c r="D33" s="0">
-        <v>1</v>
-      </c>
-      <c r="E33" s="0">
-        <v>1</v>
-      </c>
+      <c r="D33" s="0"/>
+      <c r="E33" s="0"/>
     </row>
     <row r="34">
       <c r="A34" s="0" t="s">
@@ -935,12 +887,8 @@
       <c r="C34" s="0">
         <v>1</v>
       </c>
-      <c r="D34" s="0">
-        <v>0</v>
-      </c>
-      <c r="E34" s="0">
-        <v>1</v>
-      </c>
+      <c r="D34" s="0"/>
+      <c r="E34" s="0"/>
     </row>
     <row r="35">
       <c r="A35" s="0" t="s">
@@ -952,12 +900,8 @@
       <c r="C35" s="0">
         <v>0</v>
       </c>
-      <c r="D35" s="0">
-        <v>0</v>
-      </c>
-      <c r="E35" s="0">
-        <v>1</v>
-      </c>
+      <c r="D35" s="0"/>
+      <c r="E35" s="0"/>
     </row>
     <row r="36">
       <c r="A36" s="0" t="s">
@@ -969,12 +913,8 @@
       <c r="C36" s="0">
         <v>1</v>
       </c>
-      <c r="D36" s="0">
-        <v>0</v>
-      </c>
-      <c r="E36" s="0">
-        <v>1</v>
-      </c>
+      <c r="D36" s="0"/>
+      <c r="E36" s="0"/>
     </row>
     <row r="37">
       <c r="A37" s="0" t="s">
@@ -986,12 +926,8 @@
       <c r="C37" s="0">
         <v>1</v>
       </c>
-      <c r="D37" s="0">
-        <v>0</v>
-      </c>
-      <c r="E37" s="0">
-        <v>1</v>
-      </c>
+      <c r="D37" s="0"/>
+      <c r="E37" s="0"/>
     </row>
     <row r="38">
       <c r="A38" s="0" t="s">
@@ -1003,12 +939,8 @@
       <c r="C38" s="0">
         <v>1</v>
       </c>
-      <c r="D38" s="0">
-        <v>1</v>
-      </c>
-      <c r="E38" s="0">
-        <v>1</v>
-      </c>
+      <c r="D38" s="0"/>
+      <c r="E38" s="0"/>
     </row>
     <row r="39">
       <c r="A39" s="0" t="s">
@@ -1020,12 +952,8 @@
       <c r="C39" s="0">
         <v>0</v>
       </c>
-      <c r="D39" s="0">
-        <v>0</v>
-      </c>
-      <c r="E39" s="0">
-        <v>0</v>
-      </c>
+      <c r="D39" s="0"/>
+      <c r="E39" s="0"/>
     </row>
     <row r="40">
       <c r="A40" s="0" t="s">
@@ -1037,12 +965,8 @@
       <c r="C40" s="0">
         <v>0</v>
       </c>
-      <c r="D40" s="0">
-        <v>1</v>
-      </c>
-      <c r="E40" s="0">
-        <v>0</v>
-      </c>
+      <c r="D40" s="0"/>
+      <c r="E40" s="0"/>
     </row>
     <row r="41">
       <c r="A41" s="0" t="s">
@@ -1054,12 +978,8 @@
       <c r="C41" s="0">
         <v>0</v>
       </c>
-      <c r="D41" s="0">
-        <v>1</v>
-      </c>
-      <c r="E41" s="0">
-        <v>1</v>
-      </c>
+      <c r="D41" s="0"/>
+      <c r="E41" s="0"/>
     </row>
     <row r="42">
       <c r="A42" s="0" t="s">
@@ -1071,12 +991,8 @@
       <c r="C42" s="0">
         <v>0</v>
       </c>
-      <c r="D42" s="0">
-        <v>0</v>
-      </c>
-      <c r="E42" s="0">
-        <v>1</v>
-      </c>
+      <c r="D42" s="0"/>
+      <c r="E42" s="0"/>
     </row>
     <row r="43">
       <c r="A43" s="0" t="s">
@@ -1088,12 +1004,8 @@
       <c r="C43" s="0">
         <v>0</v>
       </c>
-      <c r="D43" s="0">
-        <v>0</v>
-      </c>
-      <c r="E43" s="0">
-        <v>0</v>
-      </c>
+      <c r="D43" s="0"/>
+      <c r="E43" s="0"/>
     </row>
     <row r="44">
       <c r="A44" s="0" t="s">
@@ -1105,12 +1017,8 @@
       <c r="C44" s="0">
         <v>0</v>
       </c>
-      <c r="D44" s="0">
-        <v>1</v>
-      </c>
-      <c r="E44" s="0">
-        <v>1</v>
-      </c>
+      <c r="D44" s="0"/>
+      <c r="E44" s="0"/>
     </row>
     <row r="45">
       <c r="A45" s="0" t="s">
@@ -1122,12 +1030,8 @@
       <c r="C45" s="0">
         <v>0</v>
       </c>
-      <c r="D45" s="0">
-        <v>0</v>
-      </c>
-      <c r="E45" s="0">
-        <v>0</v>
-      </c>
+      <c r="D45" s="0"/>
+      <c r="E45" s="0"/>
     </row>
     <row r="46">
       <c r="A46" s="0" t="s">
@@ -1139,12 +1043,8 @@
       <c r="C46" s="0">
         <v>0</v>
       </c>
-      <c r="D46" s="0">
-        <v>0</v>
-      </c>
-      <c r="E46" s="0">
-        <v>1</v>
-      </c>
+      <c r="D46" s="0"/>
+      <c r="E46" s="0"/>
     </row>
     <row r="47">
       <c r="A47" s="0" t="s">
@@ -1156,12 +1056,8 @@
       <c r="C47" s="0">
         <v>0</v>
       </c>
-      <c r="D47" s="0">
-        <v>1</v>
-      </c>
-      <c r="E47" s="0">
-        <v>0</v>
-      </c>
+      <c r="D47" s="0"/>
+      <c r="E47" s="0"/>
     </row>
     <row r="48">
       <c r="A48" s="0" t="s">
@@ -1173,12 +1069,8 @@
       <c r="C48" s="0">
         <v>0</v>
       </c>
-      <c r="D48" s="0">
-        <v>1</v>
-      </c>
-      <c r="E48" s="0">
-        <v>1</v>
-      </c>
+      <c r="D48" s="0"/>
+      <c r="E48" s="0"/>
     </row>
     <row r="49">
       <c r="A49" s="0" t="s">
@@ -1190,12 +1082,8 @@
       <c r="C49" s="0">
         <v>0</v>
       </c>
-      <c r="D49" s="0">
-        <v>1</v>
-      </c>
-      <c r="E49" s="0">
-        <v>1</v>
-      </c>
+      <c r="D49" s="0"/>
+      <c r="E49" s="0"/>
     </row>
     <row r="50">
       <c r="A50" s="0" t="s">
@@ -1207,12 +1095,8 @@
       <c r="C50" s="0">
         <v>0</v>
       </c>
-      <c r="D50" s="0">
-        <v>1</v>
-      </c>
-      <c r="E50" s="0">
-        <v>0</v>
-      </c>
+      <c r="D50" s="0"/>
+      <c r="E50" s="0"/>
     </row>
     <row r="51">
       <c r="A51" s="0" t="s">
@@ -1224,12 +1108,8 @@
       <c r="C51" s="0">
         <v>0</v>
       </c>
-      <c r="D51" s="0">
-        <v>1</v>
-      </c>
-      <c r="E51" s="0">
-        <v>1</v>
-      </c>
+      <c r="D51" s="0"/>
+      <c r="E51" s="0"/>
     </row>
     <row r="52">
       <c r="A52" s="0" t="s">
@@ -1241,12 +1121,8 @@
       <c r="C52" s="0">
         <v>0</v>
       </c>
-      <c r="D52" s="0">
-        <v>0</v>
-      </c>
-      <c r="E52" s="0">
-        <v>0</v>
-      </c>
+      <c r="D52" s="0"/>
+      <c r="E52" s="0"/>
     </row>
     <row r="53">
       <c r="A53" s="0" t="s">
@@ -1258,12 +1134,8 @@
       <c r="C53" s="0">
         <v>0</v>
       </c>
-      <c r="D53" s="0">
-        <v>0</v>
-      </c>
-      <c r="E53" s="0">
-        <v>0</v>
-      </c>
+      <c r="D53" s="0"/>
+      <c r="E53" s="0"/>
     </row>
     <row r="54">
       <c r="A54" s="0" t="s">
@@ -1275,12 +1147,8 @@
       <c r="C54" s="0">
         <v>0</v>
       </c>
-      <c r="D54" s="0">
-        <v>1</v>
-      </c>
-      <c r="E54" s="0">
-        <v>1</v>
-      </c>
+      <c r="D54" s="0"/>
+      <c r="E54" s="0"/>
     </row>
     <row r="55">
       <c r="A55" s="0" t="s">
@@ -1292,12 +1160,8 @@
       <c r="C55" s="0">
         <v>0</v>
       </c>
-      <c r="D55" s="0">
-        <v>0</v>
-      </c>
-      <c r="E55" s="0">
-        <v>0</v>
-      </c>
+      <c r="D55" s="0"/>
+      <c r="E55" s="0"/>
     </row>
     <row r="56">
       <c r="A56" s="0" t="s">
@@ -1309,12 +1173,8 @@
       <c r="C56" s="0">
         <v>0</v>
       </c>
-      <c r="D56" s="0">
-        <v>0</v>
-      </c>
-      <c r="E56" s="0">
-        <v>0</v>
-      </c>
+      <c r="D56" s="0"/>
+      <c r="E56" s="0"/>
     </row>
     <row r="57">
       <c r="A57" s="0" t="s">
@@ -1326,12 +1186,8 @@
       <c r="C57" s="0">
         <v>0</v>
       </c>
-      <c r="D57" s="0">
-        <v>0</v>
-      </c>
-      <c r="E57" s="0">
-        <v>1</v>
-      </c>
+      <c r="D57" s="0"/>
+      <c r="E57" s="0"/>
     </row>
     <row r="58">
       <c r="A58" s="0" t="s">
@@ -1343,12 +1199,8 @@
       <c r="C58" s="0">
         <v>0</v>
       </c>
-      <c r="D58" s="0">
-        <v>0</v>
-      </c>
-      <c r="E58" s="0">
-        <v>0</v>
-      </c>
+      <c r="D58" s="0"/>
+      <c r="E58" s="0"/>
     </row>
     <row r="59">
       <c r="A59" s="0" t="s">
@@ -1360,12 +1212,8 @@
       <c r="C59" s="0">
         <v>0</v>
       </c>
-      <c r="D59" s="0">
-        <v>1</v>
-      </c>
-      <c r="E59" s="0">
-        <v>1</v>
-      </c>
+      <c r="D59" s="0"/>
+      <c r="E59" s="0"/>
     </row>
     <row r="60">
       <c r="A60" s="0" t="s">
@@ -1377,12 +1225,8 @@
       <c r="C60" s="0">
         <v>0</v>
       </c>
-      <c r="D60" s="0">
-        <v>1</v>
-      </c>
-      <c r="E60" s="0">
-        <v>0</v>
-      </c>
+      <c r="D60" s="0"/>
+      <c r="E60" s="0"/>
     </row>
     <row r="61">
       <c r="A61" s="0" t="s">
@@ -1394,12 +1238,8 @@
       <c r="C61" s="0">
         <v>1</v>
       </c>
-      <c r="D61" s="0">
-        <v>0</v>
-      </c>
-      <c r="E61" s="0">
-        <v>1</v>
-      </c>
+      <c r="D61" s="0"/>
+      <c r="E61" s="0"/>
     </row>
     <row r="62">
       <c r="A62" s="0" t="s">
@@ -1411,12 +1251,8 @@
       <c r="C62" s="0">
         <v>0</v>
       </c>
-      <c r="D62" s="0">
-        <v>1</v>
-      </c>
-      <c r="E62" s="0">
-        <v>0</v>
-      </c>
+      <c r="D62" s="0"/>
+      <c r="E62" s="0"/>
     </row>
     <row r="63">
       <c r="A63" s="0" t="s">
@@ -1428,12 +1264,8 @@
       <c r="C63" s="0">
         <v>0</v>
       </c>
-      <c r="D63" s="0">
-        <v>1</v>
-      </c>
-      <c r="E63" s="0">
-        <v>1</v>
-      </c>
+      <c r="D63" s="0"/>
+      <c r="E63" s="0"/>
     </row>
     <row r="64">
       <c r="A64" s="0" t="s">
@@ -1445,12 +1277,8 @@
       <c r="C64" s="0">
         <v>0</v>
       </c>
-      <c r="D64" s="0">
-        <v>1</v>
-      </c>
-      <c r="E64" s="0">
-        <v>0</v>
-      </c>
+      <c r="D64" s="0"/>
+      <c r="E64" s="0"/>
     </row>
     <row r="65">
       <c r="A65" s="0" t="s">
@@ -1462,12 +1290,8 @@
       <c r="C65" s="0">
         <v>0</v>
       </c>
-      <c r="D65" s="0">
-        <v>0</v>
-      </c>
-      <c r="E65" s="0">
-        <v>1</v>
-      </c>
+      <c r="D65" s="0"/>
+      <c r="E65" s="0"/>
     </row>
     <row r="66">
       <c r="A66" s="0" t="s">
@@ -1479,12 +1303,8 @@
       <c r="C66" s="0">
         <v>0</v>
       </c>
-      <c r="D66" s="0">
-        <v>0</v>
-      </c>
-      <c r="E66" s="0">
-        <v>0</v>
-      </c>
+      <c r="D66" s="0"/>
+      <c r="E66" s="0"/>
     </row>
     <row r="67">
       <c r="A67" s="0" t="s">
@@ -1496,12 +1316,8 @@
       <c r="C67" s="0">
         <v>0</v>
       </c>
-      <c r="D67" s="0">
-        <v>2</v>
-      </c>
-      <c r="E67" s="0">
-        <v>0</v>
-      </c>
+      <c r="D67" s="0"/>
+      <c r="E67" s="0"/>
     </row>
     <row r="68">
       <c r="A68" s="0" t="s">
@@ -1513,12 +1329,8 @@
       <c r="C68" s="0">
         <v>0</v>
       </c>
-      <c r="D68" s="0">
-        <v>1</v>
-      </c>
-      <c r="E68" s="0">
-        <v>0</v>
-      </c>
+      <c r="D68" s="0"/>
+      <c r="E68" s="0"/>
     </row>
     <row r="69">
       <c r="A69" s="0" t="s">
@@ -1530,12 +1342,8 @@
       <c r="C69" s="0">
         <v>0</v>
       </c>
-      <c r="D69" s="0">
-        <v>1</v>
-      </c>
-      <c r="E69" s="0">
-        <v>0</v>
-      </c>
+      <c r="D69" s="0"/>
+      <c r="E69" s="0"/>
     </row>
     <row r="70">
       <c r="A70" s="0" t="s">
@@ -1547,12 +1355,8 @@
       <c r="C70" s="0">
         <v>0</v>
       </c>
-      <c r="D70" s="0">
-        <v>0</v>
-      </c>
-      <c r="E70" s="0">
-        <v>0</v>
-      </c>
+      <c r="D70" s="0"/>
+      <c r="E70" s="0"/>
     </row>
     <row r="71">
       <c r="A71" s="0" t="s">
@@ -1564,12 +1368,8 @@
       <c r="C71" s="0">
         <v>0</v>
       </c>
-      <c r="D71" s="0">
-        <v>0</v>
-      </c>
-      <c r="E71" s="0">
-        <v>0</v>
-      </c>
+      <c r="D71" s="0"/>
+      <c r="E71" s="0"/>
     </row>
     <row r="72">
       <c r="A72" s="0" t="s">
@@ -1581,12 +1381,8 @@
       <c r="C72" s="0">
         <v>0</v>
       </c>
-      <c r="D72" s="0">
-        <v>0</v>
-      </c>
-      <c r="E72" s="0">
-        <v>1</v>
-      </c>
+      <c r="D72" s="0"/>
+      <c r="E72" s="0"/>
     </row>
     <row r="73">
       <c r="A73" s="0" t="s">
@@ -1598,12 +1394,8 @@
       <c r="C73" s="0">
         <v>0</v>
       </c>
-      <c r="D73" s="0">
-        <v>1</v>
-      </c>
-      <c r="E73" s="0">
-        <v>0</v>
-      </c>
+      <c r="D73" s="0"/>
+      <c r="E73" s="0"/>
     </row>
     <row r="74">
       <c r="A74" s="0" t="s">
@@ -1615,12 +1407,8 @@
       <c r="C74" s="0">
         <v>0</v>
       </c>
-      <c r="D74" s="0">
-        <v>1</v>
-      </c>
-      <c r="E74" s="0">
-        <v>1</v>
-      </c>
+      <c r="D74" s="0"/>
+      <c r="E74" s="0"/>
     </row>
     <row r="75">
       <c r="A75" s="0" t="s">
@@ -1632,12 +1420,8 @@
       <c r="C75" s="0">
         <v>0</v>
       </c>
-      <c r="D75" s="0">
-        <v>0</v>
-      </c>
-      <c r="E75" s="0">
-        <v>0</v>
-      </c>
+      <c r="D75" s="0"/>
+      <c r="E75" s="0"/>
     </row>
     <row r="76">
       <c r="A76" s="0" t="s">
@@ -1649,12 +1433,8 @@
       <c r="C76" s="0">
         <v>0</v>
       </c>
-      <c r="D76" s="0">
-        <v>0</v>
-      </c>
-      <c r="E76" s="0">
-        <v>0</v>
-      </c>
+      <c r="D76" s="0"/>
+      <c r="E76" s="0"/>
     </row>
     <row r="77">
       <c r="A77" s="0" t="s">
@@ -1666,12 +1446,8 @@
       <c r="C77" s="0">
         <v>0</v>
       </c>
-      <c r="D77" s="0">
-        <v>1</v>
-      </c>
-      <c r="E77" s="0">
-        <v>0</v>
-      </c>
+      <c r="D77" s="0"/>
+      <c r="E77" s="0"/>
     </row>
     <row r="78">
       <c r="A78" s="0" t="s">
@@ -1683,12 +1459,8 @@
       <c r="C78" s="0">
         <v>0</v>
       </c>
-      <c r="D78" s="0">
-        <v>0</v>
-      </c>
-      <c r="E78" s="0">
-        <v>1</v>
-      </c>
+      <c r="D78" s="0"/>
+      <c r="E78" s="0"/>
     </row>
     <row r="79">
       <c r="A79" s="0" t="s">
@@ -1700,12 +1472,8 @@
       <c r="C79" s="0">
         <v>0</v>
       </c>
-      <c r="D79" s="0">
-        <v>1</v>
-      </c>
-      <c r="E79" s="0">
-        <v>0</v>
-      </c>
+      <c r="D79" s="0"/>
+      <c r="E79" s="0"/>
     </row>
     <row r="80">
       <c r="A80" s="0" t="s">
@@ -1717,12 +1485,8 @@
       <c r="C80" s="0">
         <v>0</v>
       </c>
-      <c r="D80" s="0">
-        <v>1</v>
-      </c>
-      <c r="E80" s="0">
-        <v>0</v>
-      </c>
+      <c r="D80" s="0"/>
+      <c r="E80" s="0"/>
     </row>
     <row r="81">
       <c r="A81" s="0" t="s">
@@ -1734,12 +1498,8 @@
       <c r="C81" s="0">
         <v>0</v>
       </c>
-      <c r="D81" s="0">
-        <v>0</v>
-      </c>
-      <c r="E81" s="0">
-        <v>0</v>
-      </c>
+      <c r="D81" s="0"/>
+      <c r="E81" s="0"/>
     </row>
     <row r="82">
       <c r="A82" s="0" t="s">
@@ -1751,12 +1511,8 @@
       <c r="C82" s="0">
         <v>1</v>
       </c>
-      <c r="D82" s="0">
-        <v>0</v>
-      </c>
-      <c r="E82" s="0">
-        <v>1</v>
-      </c>
+      <c r="D82" s="0"/>
+      <c r="E82" s="0"/>
     </row>
     <row r="83">
       <c r="A83" s="0" t="s">
@@ -1768,12 +1524,8 @@
       <c r="C83" s="0">
         <v>1</v>
       </c>
-      <c r="D83" s="0">
-        <v>0</v>
-      </c>
-      <c r="E83" s="0">
-        <v>1</v>
-      </c>
+      <c r="D83" s="0"/>
+      <c r="E83" s="0"/>
     </row>
     <row r="84">
       <c r="A84" s="0" t="s">
@@ -1785,12 +1537,8 @@
       <c r="C84" s="0">
         <v>1</v>
       </c>
-      <c r="D84" s="0">
-        <v>0</v>
-      </c>
-      <c r="E84" s="0">
-        <v>1</v>
-      </c>
+      <c r="D84" s="0"/>
+      <c r="E84" s="0"/>
     </row>
     <row r="85">
       <c r="A85" s="0" t="s">
@@ -1802,12 +1550,8 @@
       <c r="C85" s="0">
         <v>1</v>
       </c>
-      <c r="D85" s="0">
-        <v>1</v>
-      </c>
-      <c r="E85" s="0">
-        <v>1</v>
-      </c>
+      <c r="D85" s="0"/>
+      <c r="E85" s="0"/>
     </row>
     <row r="86">
       <c r="A86" s="0" t="s">
@@ -1819,12 +1563,8 @@
       <c r="C86" s="0">
         <v>0</v>
       </c>
-      <c r="D86" s="0">
-        <v>0</v>
-      </c>
-      <c r="E86" s="0">
-        <v>0</v>
-      </c>
+      <c r="D86" s="0"/>
+      <c r="E86" s="0"/>
     </row>
     <row r="87">
       <c r="A87" s="0" t="s">
@@ -1836,12 +1576,8 @@
       <c r="C87" s="0">
         <v>0</v>
       </c>
-      <c r="D87" s="0">
-        <v>1</v>
-      </c>
-      <c r="E87" s="0">
-        <v>0</v>
-      </c>
+      <c r="D87" s="0"/>
+      <c r="E87" s="0"/>
     </row>
     <row r="88">
       <c r="A88" s="0" t="s">
@@ -1853,12 +1589,8 @@
       <c r="C88" s="0">
         <v>0</v>
       </c>
-      <c r="D88" s="0">
-        <v>0</v>
-      </c>
-      <c r="E88" s="0">
-        <v>0</v>
-      </c>
+      <c r="D88" s="0"/>
+      <c r="E88" s="0"/>
     </row>
     <row r="89">
       <c r="A89" s="0" t="s">
@@ -1870,12 +1602,8 @@
       <c r="C89" s="0">
         <v>0</v>
       </c>
-      <c r="D89" s="0">
-        <v>1</v>
-      </c>
-      <c r="E89" s="0">
-        <v>1</v>
-      </c>
+      <c r="D89" s="0"/>
+      <c r="E89" s="0"/>
     </row>
     <row r="90">
       <c r="A90" s="0" t="s">
@@ -1887,12 +1615,8 @@
       <c r="C90" s="0">
         <v>0</v>
       </c>
-      <c r="D90" s="0">
-        <v>1</v>
-      </c>
-      <c r="E90" s="0">
-        <v>1</v>
-      </c>
+      <c r="D90" s="0"/>
+      <c r="E90" s="0"/>
     </row>
     <row r="91">
       <c r="A91" s="0" t="s">
@@ -1904,12 +1628,8 @@
       <c r="C91" s="0">
         <v>0</v>
       </c>
-      <c r="D91" s="0">
-        <v>1</v>
-      </c>
-      <c r="E91" s="0">
-        <v>1</v>
-      </c>
+      <c r="D91" s="0"/>
+      <c r="E91" s="0"/>
     </row>
     <row r="92">
       <c r="A92" s="0" t="s">
@@ -1921,12 +1641,8 @@
       <c r="C92" s="0">
         <v>0</v>
       </c>
-      <c r="D92" s="0">
-        <v>1</v>
-      </c>
-      <c r="E92" s="0">
-        <v>0</v>
-      </c>
+      <c r="D92" s="0"/>
+      <c r="E92" s="0"/>
     </row>
     <row r="93">
       <c r="A93" s="0" t="s">
@@ -1938,12 +1654,8 @@
       <c r="C93" s="0">
         <v>0</v>
       </c>
-      <c r="D93" s="0">
-        <v>1</v>
-      </c>
-      <c r="E93" s="0">
-        <v>1</v>
-      </c>
+      <c r="D93" s="0"/>
+      <c r="E93" s="0"/>
     </row>
     <row r="94">
       <c r="A94" s="0" t="s">
@@ -1955,12 +1667,8 @@
       <c r="C94" s="0">
         <v>0</v>
       </c>
-      <c r="D94" s="0">
-        <v>0</v>
-      </c>
-      <c r="E94" s="0">
-        <v>1</v>
-      </c>
+      <c r="D94" s="0"/>
+      <c r="E94" s="0"/>
     </row>
     <row r="95">
       <c r="A95" s="0" t="s">

</xml_diff>